<commit_message>
:recket: Tested and deploy to board.
</commit_message>
<xml_diff>
--- a/Documents/Calculations.xlsx
+++ b/Documents/Calculations.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19815" windowHeight="7815"/>
+    <workbookView windowWidth="20490" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="ZCD Circuit" sheetId="1" r:id="rId1"/>
@@ -90,12 +90,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,13 +115,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -133,6 +126,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -141,6 +141,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -150,31 +158,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -189,6 +173,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -221,36 +212,38 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -278,181 +271,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -502,15 +495,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -521,21 +505,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -576,6 +545,30 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -587,152 +580,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -741,9 +734,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1083,8 +1073,8 @@
   <sheetPr/>
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -1110,109 +1100,121 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7">
+      <c r="B2" s="5"/>
+      <c r="C2" s="6">
         <v>250</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>220</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>200</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="8" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="8">
+        <f>232/10</f>
+        <v>23.2</v>
+      </c>
+      <c r="D4" s="8">
+        <f>232/10</f>
+        <v>23.2</v>
+      </c>
+      <c r="E4" s="8">
+        <f>232/10</f>
+        <v>23.2</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" ht="30" spans="1:6">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="9">
-        <v>9</v>
-      </c>
-      <c r="D5" s="9">
-        <v>9</v>
-      </c>
-      <c r="E5" s="9">
-        <v>9</v>
-      </c>
-      <c r="F5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="8">
+        <f>C2/C4</f>
+        <v>10.7758620689655</v>
+      </c>
+      <c r="D5" s="8">
+        <f>D2/D4</f>
+        <v>9.48275862068965</v>
+      </c>
+      <c r="E5" s="8">
+        <f>E2/E4</f>
+        <v>8.62068965517241</v>
+      </c>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="8"/>
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7">
-        <v>50</v>
-      </c>
-      <c r="D7" s="7">
+      <c r="B7" s="5"/>
+      <c r="C7" s="6">
         <v>20</v>
       </c>
-      <c r="E7" s="7">
+      <c r="D7" s="6">
         <v>20</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="E7" s="6">
+        <v>20</v>
+      </c>
+      <c r="F7" s="7" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7">
-        <v>1.4</v>
-      </c>
-      <c r="D8" s="7">
+      <c r="B8" s="5"/>
+      <c r="C8" s="6">
         <v>1.2</v>
       </c>
-      <c r="E8" s="7">
+      <c r="D8" s="6">
         <v>1.2</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="E8" s="6">
+        <v>1.2</v>
+      </c>
+      <c r="F8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="G8" t="s">
@@ -1220,121 +1222,121 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="8"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" ht="30" spans="1:7">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7">
+      <c r="B10" s="5"/>
+      <c r="C10" s="6">
         <v>1000</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="6">
         <v>1000</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>1000</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="7"/>
       <c r="G10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" ht="30" spans="1:7">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="9">
+      <c r="B11" s="5"/>
+      <c r="C11" s="8">
         <f>ROUNDUP((C10*(C8/((C5*SQRT(2))-C8))),2)</f>
-        <v>123.59</v>
-      </c>
-      <c r="D11" s="9">
+        <v>85.48</v>
+      </c>
+      <c r="D11" s="8">
         <f>ROUNDUP((D10*(D8/((D5*SQRT(2))-D8))),2)</f>
-        <v>104.1</v>
-      </c>
-      <c r="E11" s="9">
+        <v>98.28</v>
+      </c>
+      <c r="E11" s="8">
         <f>ROUNDUP((E10*(E8/((E5*SQRT(2))-E8))),2)</f>
-        <v>104.1</v>
-      </c>
-      <c r="F11" s="8"/>
+        <v>109.18</v>
+      </c>
+      <c r="F11" s="7"/>
       <c r="G11" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="9">
+      <c r="B12" s="5"/>
+      <c r="C12" s="8">
         <f>(C8^2)/C11</f>
-        <v>0.0158588882595679</v>
-      </c>
-      <c r="D12" s="9">
+        <v>0.0168460458586804</v>
+      </c>
+      <c r="D12" s="8">
         <f>(D8^2)/D11</f>
-        <v>0.0138328530259366</v>
-      </c>
-      <c r="E12" s="9">
+        <v>0.0146520146520147</v>
+      </c>
+      <c r="E12" s="8">
         <f>(E8^2)/E11</f>
-        <v>0.0138328530259366</v>
-      </c>
-      <c r="F12" s="8"/>
+        <v>0.0131892287964829</v>
+      </c>
+      <c r="F12" s="7"/>
       <c r="G12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="9">
+      <c r="B13" s="5"/>
+      <c r="C13" s="8">
         <f>((C5*SQRT(2)-C8)^2)/C10</f>
-        <v>0.128321818228198</v>
-      </c>
-      <c r="D13" s="9">
+        <v>0.197103917976677</v>
+      </c>
+      <c r="D13" s="8">
         <f>((D5*SQRT(2)-D8)^2)/D10</f>
-        <v>0.132892987052741</v>
-      </c>
-      <c r="E13" s="9">
+        <v>0.149099872076313</v>
+      </c>
+      <c r="E13" s="8">
         <f>((E5*SQRT(2)-E8)^2)/E10</f>
-        <v>0.132892987052741</v>
-      </c>
-      <c r="F13" s="8"/>
+        <v>0.120812989315943</v>
+      </c>
+      <c r="F13" s="7"/>
       <c r="G13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="8"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="8"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="8"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>